<commit_message>
nuevas zonas para pruebas
</commit_message>
<xml_diff>
--- a/Listado de Datos.xlsx
+++ b/Listado de Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\CATEDRA UPV-NOVA\PRACTICAS EN UPV 2024\PROYECTOS PRÁCTICAS\LIMPIEZA NUBES DE PUNTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Practicas_Nova\Proyectos\LimpiezaNubes\sample_data\Nova_RPAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180618AA-3D7E-49AB-BF12-EEB42D66EC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB02861C-8EC9-465B-8DAB-7BC0CBB3E793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
   <si>
     <t>Cultivo</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>Nombre Nube de Puntos</t>
+  </si>
+  <si>
+    <t>Zona 004</t>
+  </si>
+  <si>
+    <t>Zona 005</t>
+  </si>
+  <si>
+    <t>Zona 006</t>
+  </si>
+  <si>
+    <t>Zona 007</t>
+  </si>
+  <si>
+    <t>Zona 008</t>
   </si>
 </sst>
 </file>
@@ -181,21 +196,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -213,16 +228,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -504,33 +509,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="4" t="s">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
@@ -556,8 +561,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -582,8 +587,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -608,8 +613,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -634,58 +639,138 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="4"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -694,8 +779,8 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="4"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -709,14 +794,14 @@
     <mergeCell ref="D4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:J15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"SÍ"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"SÍ"</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>